<commit_message>
Clean Kairos data, no errors but need to manually compare to their raw report
</commit_message>
<xml_diff>
--- a/00_raw_data/Kairos_data_flags.xlsx
+++ b/00_raw_data/Kairos_data_flags.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sea/PycharmProjects/CRF22_Airplanes/00_raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A46D014-A592-A941-A240-847E7BEB2A92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3BFCD8-A1EE-DC4E-9F35-5487B3544650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37020" yWindow="1620" windowWidth="27240" windowHeight="16440" xr2:uid="{4F6C16A2-2230-A643-A873-A09C5AD33A9A}"/>
+    <workbookView xWindow="4120" yWindow="4100" windowWidth="27240" windowHeight="16440" xr2:uid="{4F6C16A2-2230-A643-A873-A09C5AD33A9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="17">
   <si>
     <t>Kairos Flag for Dropped Passes or Uncertain Rate Quantification</t>
   </si>
@@ -86,6 +86,30 @@
   </si>
   <si>
     <t>Glare</t>
+  </si>
+  <si>
+    <t>KA-1</t>
+  </si>
+  <si>
+    <t>KA-2</t>
+  </si>
+  <si>
+    <t>Partial detection</t>
+  </si>
+  <si>
+    <t>KA-3</t>
+  </si>
+  <si>
+    <t>Lower detection cutoff</t>
+  </si>
+  <si>
+    <t>KA-4</t>
+  </si>
+  <si>
+    <t>Excessive methane pooling</t>
+  </si>
+  <si>
+    <t>KA-5</t>
   </si>
 </sst>
 </file>
@@ -523,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E505FE6F-0682-7548-A96E-CD00DA9CB5D4}">
-  <dimension ref="A1:C528"/>
+  <dimension ref="A1:H528"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -534,7 +558,7 @@
     <col min="1" max="1" width="26.6640625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,79 +567,109 @@
         <v>Kairos Flag for Dropped Passes or Uncertain Rate Quantification</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="C2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="C3" t="str">
         <v>Plane deviated from flightline</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C4" t="str">
         <v>PARTIAL DETECTION</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="C5" t="str">
         <v>Cutoff - low confidence quantification</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="C6" t="str">
         <v>Excessive methane pooling near site</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="C7" t="str">
         <v>Excessive methane pooling over site</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="C8" t="str">
         <v xml:space="preserve">Excessive methane pooling over site
 </v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="C9" t="str">
         <v>Plane deviated from flightpath</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="C10" t="str">
         <v>Glare</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>2</v>
       </c>

</xml_diff>